<commit_message>
version 1.5 with feature of flask user-interface is added
</commit_message>
<xml_diff>
--- a/outputs/internshala-analytics-jobs.xlsx
+++ b/outputs/internshala-analytics-jobs.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -508,42 +508,42 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Devavi Media</t>
+          <t>8Views</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://instagram.com/devavimeida</t>
+          <t>http://www.8views.com/</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Devavi Media is a dynamic advertising agency specializing in social media management, content creation, and performance marketing. As a team that views itself as a true partner to its clients, we focus on collaborating with small, select entrepreneurs, helping them scale their businesses with tailored strategies and creative solutions. Join us in empowering businesses to grow and succeed!</t>
+          <t>8Views is a fast-paced, end-to-end digital marketing company providing solutions across digital platforms. The core focus of the company is to help brands meet their business goals through the rapidly growing online space. Our solutions include search engine optimization, social media marketing, email marketing, ad campaigns, content marketing, analytics, and more.</t>
         </is>
       </c>
       <c r="D2" t="n">
         <v>2</v>
       </c>
       <c r="E2" t="n">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Hiring since January 2025</t>
+          <t>Hiring since March 2023</t>
         </is>
       </c>
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>English Proficiency (Spoken), English Proficiency (Written), Facebook Ads, Google AdWords, Google Analytics, Certificate,  Letter of recommendation,  Job offer</t>
+          <t>Digital Advertising, Digital Marketing, Facebook Ads, Google AdWords, Google Analytics, Instagram Marketing, Search Engine Marketing (SEM), Certificate,  Letter of recommendation,  Informal dress code,  5 days a week,  Free snacks &amp; beverages</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>59</v>
+        <v>0</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Work from home</t>
+          <t>Secunderabad, Hyderabad, Madhapur, Telangana</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
@@ -553,55 +553,51 @@
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>₹ 7,500 /month</t>
+          <t>₹ 8,000 - 15,000 /month</t>
         </is>
       </c>
       <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-performance-marketing-internship-at-devavi-media1744000662</t>
+          <t>https://internshala.com/internship/detail/performance-marketing-paid-ads-internship-in-multiple-locations-at-8views1744015239</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Myla Organics</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>http://mylaorganics.com</t>
-        </is>
-      </c>
+          <t>MentorBoxx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Myla Organics is a cutting-edge software development company dedicated to creating innovative solutions that empower businesses and individuals. With a strong focus on organic growth and sustainability, we harness the latest technologies to build custom software products tailored to our clients' unique needs. Our team of experienced developers, designers, and project managers collaborates closely with clients to understand their objectives and deliver high-quality, scalable, and user-friendly software solutions. Whether it's web development, mobile apps, or enterprise software, we leverage our expertise to drive digital transformation and help our clients stay ahead in today's competitive landscape. At Myla Organics, we prioritize sustainability and ethical practices in everything we do.</t>
+          <t>Our sole aim at MentorBoxx is to bridge the gap between universities &amp; industries. We select 30 students every month to regularly interact with the right industry experts, work on live industry projects, and grasp as much industry knowledge as possible.</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="E3" t="n">
-        <v>24</v>
+        <v>1630</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Hiring since April 2024</t>
+          <t>Hiring since April 2021</t>
         </is>
       </c>
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Data Science, Machine Learning, Certificate,  Letter of recommendation,  Flexible work hours,  5 days a week,  Job offer</t>
+          <t>Creative Writing, Email Marketing, English Proficiency (Spoken), English Proficiency (Written), Facebook Marketing, Google AdWords, Google Analytics, Instagram Marketing, Search Engine Marketing (SEM), Search Engine Optimization (SEO), Certificate,  Flexible work hours</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>1000</v>
+        <v>208</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Work from home</t>
+          <t>Chennai, Coimbatore, Delhi, Gurgaon, Lucknow, Patna, Pune, Ranchi, Hyderabad, Mumbai, Varanasi, Jaipur, Noida, Bangalore, Andhra Tharhi</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
@@ -611,43 +607,47 @@
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>₹ 5,000 - 7,000 /month</t>
+          <t>₹ 10,000 /month</t>
         </is>
       </c>
       <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-part-time-data-science-internship-at-myla-organics1743823512</t>
+          <t>https://internshala.com/internship/detail/part-time-digital-marketing-internship-in-multiple-locations-at-mentorboxx1744029239</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Renan Partners</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
+          <t>Vitals7</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>http://vitals7.com</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Renan is an AI consultancy organization that offers data annotation and LLM fine-tuning services across over 50 languages.</t>
+          <t>Vitals7 is an innovative telehealth and AI-driven self-health monitoring platform. We empower users with cutting-edge technology, predictive analytics, and holistic healthcare solutions. Our platform integrates IoT-based health monitoring, AI-powered analytics, and digital health consultations to make healthcare more accessible and affordable. We are looking for passionate and creative digital marketing interns to join our team and help execute AI-powered marketing campaigns using the latest automation tools.</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Hiring since August 2024</t>
+          <t>Hiring since March 2025</t>
         </is>
       </c>
       <c r="G4" t="inlineStr"/>
       <c r="H4" t="inlineStr">
         <is>
-          <t>MySQL, Python, Certificate,  Letter of recommendation,  Flexible work hours,  5 days a week,  Job offer</t>
+          <t>Django, Flask, Machine Learning, Python, Certificate,  Letter of recommendation,  Flexible work hours</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -655,7 +655,7 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Work from home</t>
+          <t>Hyderabad, Bangalore                                                    (Hybrid)</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
@@ -665,52 +665,51 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>₹ 5,000 /month</t>
+          <t>₹ 10,000 - 40,000 /month</t>
         </is>
       </c>
       <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-data-analyst-internship-at-renan-partners1743678766</t>
+          <t>https://internshala.com/internship/detail/python-development-internship-in-multiple-locations-at-vitals71743684810</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Big Bulls</t>
+          <t>Tex N Co</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>At Big Bulls, our aim is simple: to educate you on profitable money investment. Whether you've considered becoming a trader, what to trade, which trading software to use, or how to understand the market, look no further. Our trading program offers a comprehensive range of financial training courses focused on price action trading. Whether you're interested in trading futures markets, commodities, or day trading currency markets, we can teach you how to trade consistently and profitably.
-At Training Traders, we believe we provide the best training, coaching, and mentorship available anywhere. Your training course marks just the beginning of your journey with us. We prioritize offering robust mentorship and coaching follow-up because the education process never truly ends, regardless of whether you're a novice or an experienced trader. In the ever-changing market landscape, traders learn something new every day.</t>
+          <t>We are an interior design and construction firm handling design and execution for both residential and commercial interior, construction, and renovation projects.</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>564</v>
+        <v>9</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Hiring since June 2024</t>
+          <t>Hiring since July 2021</t>
         </is>
       </c>
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Effective Communication, Certificate,  Letter of recommendation,  5 days a week,  Job offer</t>
+          <t>AutoCAD, Data Analytics, Engineering Drawing, Engineering Surveying, English Proficiency (Written), Google Docs, Google Sheets, Google SketchUp , Certificate,  Letter of recommendation,  Informal dress code,  Free snacks &amp; beverages</t>
         </is>
       </c>
       <c r="I5" t="n">
-        <v>1000</v>
+        <v>106</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Work from home</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
@@ -720,51 +719,51 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>₹ 8,000 - 30,000 /month</t>
+          <t>₹ 10,000 /month</t>
         </is>
       </c>
       <c r="M5" t="inlineStr"/>
       <c r="N5" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-part-time-technical-research-internship-at-big-bulls1743587824</t>
+          <t>https://internshala.com/internship/detail/technical-assistant-internship-in-hyderabad-at-tex-n-co1743582036</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DeepThought Edutech Ventures Private Limited</t>
+          <t>J K Arts</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>DeepThought (DT), a DeepTech product innovation company, dreams of transforming every school/college into an MIT/Harvard/IISER-style research institution by 2030. Our SD LMS (Socratic dialogue learning management system) is based on DT's thread-building technology. DT (SD LMS) helps product startups in grooming beginners for product-innovation roles. Some of our early clients are Kringle.ai (loyalty programs), Growpital (agri-tech), and IPx (fintech). In the long term, we'd like to serve schools, colleges, corporations, and institutions with a research and innovation culture. DT is funded by 5 school leaders, 3 parents, and 3 technologists including Mr. S.Vishwanathan (former CPO, NIIT Technologies), Mr. Anup Kalbalia (former lead, CodeChef), and Dr. Jyothi Reddy (Director of Education, The Shriram Universal School).</t>
+          <t>We are a startup, mainly focused on sentimental analysis, PR activities, and reputation management.</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>437</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>1755</v>
+        <v>1</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Hiring since March 2020</t>
+          <t>Hiring since March 2025</t>
         </is>
       </c>
       <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Data Analysis, Certificate,  Job offer</t>
+          <t>Adobe After Effects, Adobe Illustrator, Adobe Photoshop, Adobe Premiere Pro, Business Development, Client Relationship, Conflict Management, Content Management, Critical thinking, Data Analysis, Data Extraction, Data Manipulation, Final Cut Pro, Influencer Marketing, Problem Solving, Report Generation, Research and Analytics, Resource Management, Video Editing, Videography, Certificate</t>
         </is>
       </c>
       <c r="I6" t="n">
-        <v>1000</v>
+        <v>32</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Work from home</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
@@ -774,55 +773,55 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>₹ 2,000 /month</t>
+          <t>₹ 8,000 - 12,000 /month</t>
         </is>
       </c>
       <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-part-time-data-analytics-internship-at-deepthought-edutech-ventures-private-limited1743305368</t>
+          <t>https://internshala.com/internship/detail/associate-consultant-internship-in-hyderabad-at-j-k-arts1743423990</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Knowledge Sourcing Intelligence</t>
+          <t>The Affordable Organic Store</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://www.knowledge-sourcing.com</t>
+          <t>https://theaffordableorganicstore.com/</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Knowledge Sourcing Intelligence is a market research company based in Noida, specializing in syndicated and custom market research reports. We publish research studies spanning over ten industry verticals.</t>
+          <t>We are a bunch of enthusiasts who want to make good food affordable again by cutting out the middlemen. We want to set an example that a sustainable business can also be run without exploiting the consumers with high prices. We will be successful if everyone in the country starts doing what we do. We will change the rules of retail and modern trade. We will bring the power back to the producers from the retailers or middlemen. From our team, we want only the best. We are a tech-driven company with a focus on constant innovation. We need smart people with the best analytical and communication skills and a great heart. If we succeed, we will create a world order where everyone has access to good food and will lead a content life. We promise that we will take care of you at all times.</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>91</v>
+        <v>156</v>
       </c>
       <c r="E7" t="n">
-        <v>121</v>
+        <v>714</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Hiring since January 2016</t>
+          <t>Hiring since May 2020</t>
         </is>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Economics, English Proficiency (Spoken), English Proficiency (Written), MS-Excel, MS-Office, MS-PowerPoint, MS-Word, Research and Analytics, Certificate,  5 days a week,  Job offer</t>
+          <t>Data Analytics, Data Science, MS-Excel, MS-Office, Power BI, SQL, Certificate,  Letter of recommendation</t>
         </is>
       </c>
       <c r="I7" t="n">
-        <v>459</v>
+        <v>226</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Work from home</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
@@ -832,55 +831,55 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>₹ 10,000 /month</t>
+          <t>₹ 5,000 /month</t>
         </is>
       </c>
       <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-market-research-internship-at-knowledge-sourcing-intelligence1742900377</t>
+          <t>https://internshala.com/internship/detail/data-analytics-internship-in-hyderabad-at-the-affordable-organic-store1742636460</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Rapidalley</t>
+          <t>RIAI</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.rapidalley.com/</t>
+          <t>https://riai.co.in/</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Rapidalley is a service-oriented company. We provide our clients with technical solutions to upgrade their businesses. We value digital recognition and aesthetic appeal. Our mission is to assist all businesses, from little shops to giant enterprises, in building their online presence and establishing their brand identity. Our expertise includes website development, graphic design and branding, products and packaging, social media, and ad campaigns.</t>
+          <t>At RIAI, we are not just developing AI; we are redefining how AI interacts with users and businesses through continuous research and development.</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>61</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>81</v>
+        <v>5</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Hiring since July 2020</t>
+          <t>Hiring since March 2025</t>
         </is>
       </c>
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Business Research, Design Thinking, Effective Communication, English Proficiency (Spoken), English Proficiency (Written), MS-Excel, MS-Office, Research and Analytics, Certificate,  Letter of recommendation,  Flexible work hours,  5 days a week,  Job offer</t>
+          <t>Email Marketing, Facebook Ads, Google AdWords, Google Analytics, Search Engine Optimization (SEO), WordPress, Certificate,  Letter of recommendation</t>
         </is>
       </c>
       <c r="I8" t="n">
-        <v>582</v>
+        <v>65</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Work from home</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
@@ -890,51 +889,51 @@
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>₹ 3,000-7,500 /month</t>
+          <t>₹ 18,000 /month</t>
         </is>
       </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-market-research-internship-at-rapidalley1742548980</t>
+          <t>https://internshala.com/internship/detail/psychology-behavioral-marketing-strategic-communications-internship-in-hyderabad-at-riai1742462010</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Emoolar Technology Private Limited</t>
+          <t>Grow Easy Hair Care Solutions Private Limited</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>At Emoolar, we are a leading provider of comprehensive IT services tailored to meet the evolving needs of businesses in the digital age. With a commitment to excellence and innovation, we deliver cutting-edge solutions that empower organizations to thrive in today's dynamic and competitive landscape.</t>
+          <t>We are a startup in the hair care industry working to overcome problems of traditional hair care methods and provide chemical-free products to customers.</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E9" t="n">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Hiring since August 2021</t>
+          <t>Hiring since March 2021</t>
         </is>
       </c>
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Data Analytics, Certificate,  Letter of recommendation,  Flexible work hours,  5 days a week,  Job offer</t>
+          <t>Data Analytics, Research and Analytics, Certificate,  Letter of recommendation,  Informal dress code,  Free snacks &amp; beverages,  Job offer</t>
         </is>
       </c>
       <c r="I9" t="n">
-        <v>1000</v>
+        <v>86</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Work from home</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
@@ -944,55 +943,55 @@
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>₹ 5,000 /month</t>
+          <t>₹ 2,000 /month</t>
         </is>
       </c>
       <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-part-time-data-analytics-internship-at-emoolar-technology-private-limited1742470264</t>
+          <t>https://internshala.com/internship/detail/business-analytics-internship-in-hyderabad-at-grow-easy-hair-care-solutions-private-limited1742447585</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>MyFitFuel (Inventiva Labs Private Limited)</t>
+          <t>APTAGRIM CONSULTING PRIVATE LIMITED</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://www.myfitfuel.in</t>
+          <t>https://aptagrim.com/</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>MyFitFuel is a sports &amp; fitness nutrition startup with a long-term vision of solving some of the very important problems in the sports &amp; fitness nutrition industry in India. We have a growing number of happy customers who love our products and always look towards our brand with trust which brings better quality nutrition &amp; knowledge for their fitness goals. With the help of a hard-working and smart working team, we aim to bring wonderful experiences to our customers. We are based in South Delhi.</t>
+          <t>APTAGRIM CONSULTING PRIVATE LIMITED is a DeepTech AI company that offers a range of AI services to businesses across different industries. With expertise in deep learning, CNN, computer vision, NLP, and chatbot development, Aptagrim provides AI-powered solutions that automate business processes, analyze data, and enhance customer engagement. The company also offers data engineering and business intelligence services that turn data into actionable insights. Aptagrim is equipped to handle product engineering services, incubate ideas, and develop MVPs for startups and entrepreneurs.</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="E10" t="n">
-        <v>38</v>
+        <v>124</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Hiring since October 2016</t>
+          <t>Hiring since March 2023</t>
         </is>
       </c>
       <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Digital Marketing, Email Marketing, English Proficiency (Written), MS-Excel, Certificate,  Letter of recommendation,  Flexible work hours,  Job offer</t>
+          <t>Computer Vision, Deep Learning, Natural Language Processing (NLP), Certificate,  Letter of recommendation,  5 days a week,  Free snacks &amp; beverages</t>
         </is>
       </c>
       <c r="I10" t="n">
-        <v>91</v>
+        <v>674</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Work from home</t>
+          <t>Hyderabad</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
@@ -1002,13 +1001,287 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>₹ 6,000-7,000 /month</t>
+          <t>₹ 15,000 /month</t>
         </is>
       </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
-          <t>https://internshala.com/internship/detail/work-from-home-digital-marketing-internship-at-myfitfuel-inventiva-labs-private-limited1741679541</t>
+          <t>https://internshala.com/internship/detail/ai-engineer-internship-in-hyderabad-at-aptagrim-consulting-private-limited1742035373</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Denary Media Private Limited</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>We are a relatively new company based out of Secunderabad. Our founders have been in the digital space for over 6 years and are quite adept at delivering data-driven results. We are currently working with two large hospital chains and a few other large brands in Hyderabad.</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>30</v>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Hiring since October 2019</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Digital Marketing, English Proficiency (Written), Google Analytics, Search Engine Optimization (SEO), Certificate</t>
+        </is>
+      </c>
+      <c r="I11" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Hyderabad</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>Stipend</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>₹ 10,000 /month</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/search-engine-optimization-seo-internship-in-hyderabad-at-denary-media-private-limited1741765638</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Megaminds IT Services</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>We provide application solutions and development needs to clients. We offer business solutions for computing and creative excellence and deliver innovative and cost-effective solutions with ethics. Our experienced and committed team, with its strong focus on technology, is the backbone of our company in delivering the synergy of creative solutions. We design, develop, and deliver cost-effective and high-quality software applications. We provide e-commerce, retail, manufacturing, and many other services. We work on political campaigning with transparency. Megaminds IT Services (now Megaminds IT &amp; Job Consultancy Services) has started job consultancy services too.</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>81</v>
+      </c>
+      <c r="E12" t="n">
+        <v>304</v>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Hiring since March 2019</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Algorithms, Business Analysis, Computer Vision, Data Analysis, Data Analytics, Data Science, English Proficiency (Spoken), English Proficiency (Written), LaTeX, Machine Learning, MS-PowerPoint, MS-Word, Power BI, Research and Analytics, Certificate,  Letter of recommendation</t>
+        </is>
+      </c>
+      <c r="I12" t="n">
+        <v>178</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Hyderabad</t>
+        </is>
+      </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>Stipend</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>₹ 6,000-8,000 /month</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/content-writer-internship-in-hyderabad-at-megaminds-it-services1741669406</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LYWO Recruitment Consulting LLP</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>LYWO is an early-stage start-up with the objective to identify or develop an AI-assisted behavioral model that is simple enough to be used by an organization of any size.</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>7</v>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Hiring since March 2025</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Adobe After Effects, Adobe Creative Suite, Adobe Illustrator, Adobe InDesign, Adobe Photoshop, Adobe Photoshop Lightroom CC, Adobe Premiere Pro, Computer Vision, Visual Basic (VB), Certificate,  Letter of recommendation,  Job offer</t>
+        </is>
+      </c>
+      <c r="I13" t="n">
+        <v>134</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Hyderabad</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>Stipend</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>₹ 15,000 /month</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/graphic-design-internship-in-hyderabad-at-lywo-recruitment-consulting-llp1741585446</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>The Short Media</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>https://theshortmedia.com/</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>The Short Media is a marketing agency specializing in short-form video and social commerce. Founded by former TikTok leaders who shaped the platform's advertising landscape, we bring a unique blend of innovation and expertise to our clients. Our team has a proven track record of driving exceptional results, having managed substantial ad budgets and developed groundbreaking strategies. We empower brands to connect with their audiences on TikTok, Meta, Snap, and social e-commerce, ensuring they stay ahead in the ever-evolving digital marketplace.</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1</v>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Hiring since March 2025</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Data Analytics, Digital Marketing, Facebook Ads, Marketing, Job offer</t>
+        </is>
+      </c>
+      <c r="I14" t="n">
+        <v>339</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Hyderabad</t>
+        </is>
+      </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>Stipend</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>₹ 30,000 /month</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/performance-marketing-specialist-internship-in-hyderabad-at-the-short-media1741255003</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Medstown Private Limited</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>At Medstown our mission is to provide each customer with seamless and fast medicine delivery services, while not only saving their money and time but also uplifting and supporting our local pharmacies. We at Medstown aim to be the one stop shop and go to solution for patients in need of medicines, while ensuring our local pharmacies grow too. This way we aim to create a win-win situation for both customer and supplier.</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>13</v>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Hiring since September 2023</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Data Analysis, Effective Communication, Negotiation, Problem Solving, Time Management, Job offer</t>
+        </is>
+      </c>
+      <c r="I15" t="n">
+        <v>177</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Hyderabad</t>
+        </is>
+      </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>Stipend</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>₹ 10,000 /month</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>https://internshala.com/internship/detail/customer-success-internship-in-hyderabad-at-medstown-private-limited1741005176</t>
         </is>
       </c>
     </row>

</xml_diff>